<commit_message>
Update CMS FOR LED 的调整（LEIVS北京蓝色港湾店）20191107.xlsx
</commit_message>
<xml_diff>
--- a/2019/北京蓝色港湾店/05 系统集成/LED信息/CMS FOR LED 的调整（LEIVS北京蓝色港湾店）20191107.xlsx
+++ b/2019/北京蓝色港湾店/05 系统集成/LED信息/CMS FOR LED 的调整（LEIVS北京蓝色港湾店）20191107.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\File Server\Tree Sapling\03 Levi's\gitCube-levisProject\2019\北京蓝色港湾店\05 系统集成\LED信息\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C0DD5C-2800-4766-952F-ADE2AB228554}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED6ABB54-2AAE-4A42-962F-073B5AED2FDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="972" yWindow="-108" windowWidth="22176" windowHeight="14616" tabRatio="805" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="972" yWindow="-108" windowWidth="22176" windowHeight="14616" tabRatio="805" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="屏幕分割" sheetId="7" r:id="rId1"/>
@@ -259,7 +259,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="176" formatCode="?.#&quot;个&quot;"/>
-    <numFmt numFmtId="178" formatCode="0_ "/>
+    <numFmt numFmtId="177" formatCode="0_ "/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -575,7 +575,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1">
       <alignment vertical="center"/>
@@ -600,35 +600,9 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3"/>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="7" fillId="3" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="10" fillId="3" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -638,35 +612,7 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -681,32 +627,89 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="9" fillId="3" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="3" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="10" fillId="0" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="10" fillId="0" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="10" fillId="0" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="10" fillId="0" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1158,7 +1161,7 @@
               <a:cs typeface="+mn-cs"/>
               <a:sym typeface="Helvetica"/>
             </a:rPr>
-            <a:t>STB1(1152*1080)</a:t>
+            <a:t>STB1(1144*1080)</a:t>
           </a:r>
           <a:endParaRPr kumimoji="0" lang="zh-CN" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
@@ -2259,7 +2262,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0840242B-9A89-4F4D-93E8-1F02C65A3D0D}">
   <dimension ref="A1:IP10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I4" sqref="I4:I6"/>
     </sheetView>
   </sheetViews>
@@ -2288,270 +2291,254 @@
       <c r="M1" s="9"/>
     </row>
     <row r="2" spans="1:250" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="14" t="s">
+      <c r="B2" s="47"/>
+      <c r="C2" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="16" t="s">
+      <c r="D2" s="49"/>
+      <c r="E2" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="17" t="s">
+      <c r="I2" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="16" t="s">
+      <c r="J2" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="16" t="s">
+      <c r="K2" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="16"/>
+      <c r="L2" s="43"/>
       <c r="IP2" s="11"/>
     </row>
     <row r="3" spans="1:250" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="19"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
       <c r="IP3" s="11"/>
     </row>
     <row r="4" spans="1:250" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="D4" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="46">
+      <c r="E4" s="25">
         <v>1</v>
       </c>
-      <c r="F4" s="46">
+      <c r="F4" s="25">
         <v>1</v>
       </c>
-      <c r="G4" s="46">
+      <c r="G4" s="25">
         <v>1</v>
       </c>
-      <c r="H4" s="46">
+      <c r="H4" s="25">
         <v>1</v>
       </c>
-      <c r="I4" s="46" t="s">
+      <c r="I4" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="J4" s="28"/>
-      <c r="K4" s="49" t="s">
+      <c r="J4" s="27"/>
+      <c r="K4" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="L4" s="26"/>
+      <c r="L4" s="45"/>
       <c r="IP4" s="11"/>
     </row>
     <row r="5" spans="1:250" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="36"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="48"/>
-      <c r="I5" s="48"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="50"/>
-      <c r="L5" s="26"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="33"/>
+      <c r="L5" s="45"/>
       <c r="IP5" s="11"/>
     </row>
     <row r="6" spans="1:250" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="43"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="47"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="51"/>
-      <c r="L6" s="26"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="45"/>
       <c r="IP6" s="11"/>
     </row>
     <row r="7" spans="1:250" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="35" t="s">
+      <c r="D7" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="46">
+      <c r="E7" s="25">
         <v>1</v>
       </c>
-      <c r="F7" s="46">
+      <c r="F7" s="25">
         <v>1</v>
       </c>
-      <c r="G7" s="46">
+      <c r="G7" s="25">
         <v>1</v>
       </c>
-      <c r="H7" s="46">
+      <c r="H7" s="25">
         <v>1</v>
       </c>
-      <c r="I7" s="46" t="s">
+      <c r="I7" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="J7" s="31"/>
-      <c r="K7" s="32"/>
-      <c r="L7" s="26"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="35"/>
+      <c r="L7" s="45"/>
       <c r="IP7" s="11"/>
     </row>
     <row r="8" spans="1:250" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="43"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="47"/>
-      <c r="I8" s="47"/>
-      <c r="J8" s="33"/>
-      <c r="K8" s="34"/>
-      <c r="L8" s="26"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="45"/>
       <c r="IP8" s="11"/>
     </row>
     <row r="9" spans="1:250" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="27" t="s">
+      <c r="D9" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="45">
+      <c r="E9" s="24">
         <v>1</v>
       </c>
-      <c r="F9" s="45">
+      <c r="F9" s="24">
         <v>1</v>
       </c>
-      <c r="G9" s="45">
+      <c r="G9" s="24">
         <v>1</v>
       </c>
-      <c r="H9" s="45">
+      <c r="H9" s="24">
         <v>1</v>
       </c>
-      <c r="I9" s="27" t="s">
+      <c r="I9" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="J9" s="42"/>
-      <c r="K9" s="25"/>
-      <c r="L9" s="26"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="45"/>
       <c r="IP9" s="11"/>
     </row>
     <row r="10" spans="1:250" ht="15.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="37"/>
-      <c r="B10" s="38"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="44">
+      <c r="A10" s="17"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="23">
         <f>SUM(E4:E9)</f>
         <v>3</v>
       </c>
-      <c r="F10" s="39">
+      <c r="F10" s="19">
         <f>SUM(F4:F9)</f>
         <v>3</v>
       </c>
-      <c r="G10" s="39">
+      <c r="G10" s="19">
         <f>SUM(G4:G9)</f>
         <v>3</v>
       </c>
-      <c r="H10" s="39">
+      <c r="H10" s="19">
         <f>SUM(H4:H9)</f>
         <v>3</v>
       </c>
-      <c r="I10" s="40"/>
-      <c r="J10" s="40"/>
-      <c r="K10" s="40"/>
-      <c r="L10" s="41"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="21"/>
       <c r="IP10" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J4:J6"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K4:K6"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="I4:I6"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="G4:G6"/>
-    <mergeCell ref="H4:H6"/>
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="J2:J3"/>
     <mergeCell ref="K2:K3"/>
@@ -2562,6 +2549,22 @@
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="H2:H3"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J4:J6"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K4:K6"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="I4:I6"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2631,7 +2634,7 @@
   <dimension ref="B1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="D2" sqref="C2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2671,10 +2674,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B2:D4"/>
+  <dimension ref="B2:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2686,12 +2689,12 @@
     <col min="6" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="2">
         <v>1088</v>
       </c>
     </row>
-    <row r="3" spans="2:4" ht="138" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:5" ht="138" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2">
         <v>1152</v>
       </c>
@@ -2699,13 +2702,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E5" s="52"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>